<commit_message>
added one column coin flips
</commit_message>
<xml_diff>
--- a/MuenzwurfAlle.xlsx
+++ b/MuenzwurfAlle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neuwirth/SalzburgLV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CE730B-E8E4-804B-BD90-99A5B02CF67A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB0507E-A643-CF49-BA10-3FE8E0995EBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="1820" windowWidth="30220" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,8 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3638" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3839" uniqueCount="45">
   <si>
     <t>k</t>
   </si>
@@ -161,12 +159,21 @@
   <si>
     <t>Spasojevic</t>
   </si>
+  <si>
+    <t>Rothschadl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> k</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> z</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +185,12 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -201,10 +214,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,15 +557,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N201"/>
+  <dimension ref="A1:O201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="F203" sqref="F203"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -594,8 +608,11 @@
       <c r="N1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -638,8 +655,11 @@
       <c r="N2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -682,8 +702,11 @@
       <c r="N3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -726,8 +749,11 @@
       <c r="N4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -770,8 +796,11 @@
       <c r="N5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -814,8 +843,11 @@
       <c r="N6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -858,8 +890,11 @@
       <c r="N7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -902,8 +937,11 @@
       <c r="N8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -946,8 +984,11 @@
       <c r="N9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -990,8 +1031,11 @@
       <c r="N10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1034,8 +1078,11 @@
       <c r="N11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1078,8 +1125,11 @@
       <c r="N12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1122,8 +1172,11 @@
       <c r="N13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1166,8 +1219,11 @@
       <c r="N14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1210,8 +1266,11 @@
       <c r="N15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1254,8 +1313,11 @@
       <c r="N16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1298,8 +1360,11 @@
       <c r="N17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1342,8 +1407,11 @@
       <c r="N18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1386,8 +1454,11 @@
       <c r="N19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1430,8 +1501,11 @@
       <c r="N20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1474,8 +1548,11 @@
       <c r="N21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1518,8 +1595,11 @@
       <c r="N22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1562,8 +1642,11 @@
       <c r="N23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1606,8 +1689,11 @@
       <c r="N24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1650,8 +1736,11 @@
       <c r="N25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1694,8 +1783,11 @@
       <c r="N26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1738,8 +1830,11 @@
       <c r="N27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1782,8 +1877,11 @@
       <c r="N28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1826,8 +1924,11 @@
       <c r="N29" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1870,8 +1971,11 @@
       <c r="N30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1914,8 +2018,11 @@
       <c r="N31" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1958,8 +2065,11 @@
       <c r="N32" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2002,8 +2112,11 @@
       <c r="N33" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2046,8 +2159,11 @@
       <c r="N34" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2090,8 +2206,11 @@
       <c r="N35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2134,8 +2253,11 @@
       <c r="N36" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2178,8 +2300,11 @@
       <c r="N37" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2222,8 +2347,11 @@
       <c r="N38" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2266,8 +2394,11 @@
       <c r="N39" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -2310,8 +2441,11 @@
       <c r="N40" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2354,8 +2488,11 @@
       <c r="N41" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -2398,8 +2535,11 @@
       <c r="N42" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2442,8 +2582,11 @@
       <c r="N43" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2486,8 +2629,11 @@
       <c r="N44" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2530,8 +2676,11 @@
       <c r="N45" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -2574,8 +2723,11 @@
       <c r="N46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2618,8 +2770,11 @@
       <c r="N47" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -2662,8 +2817,11 @@
       <c r="N48" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -2706,8 +2864,11 @@
       <c r="N49" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2750,8 +2911,11 @@
       <c r="N50" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2794,8 +2958,11 @@
       <c r="N51" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2838,8 +3005,11 @@
       <c r="N52" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2882,8 +3052,11 @@
       <c r="N53" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -2926,8 +3099,11 @@
       <c r="N54" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -2970,8 +3146,11 @@
       <c r="N55" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -3014,8 +3193,11 @@
       <c r="N56" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -3058,8 +3240,11 @@
       <c r="N57" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -3102,8 +3287,11 @@
       <c r="N58" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3146,8 +3334,11 @@
       <c r="N59" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -3190,8 +3381,11 @@
       <c r="N60" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -3234,8 +3428,11 @@
       <c r="N61" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -3278,8 +3475,11 @@
       <c r="N62" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -3322,8 +3522,11 @@
       <c r="N63" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -3366,8 +3569,11 @@
       <c r="N64" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -3410,8 +3616,11 @@
       <c r="N65" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -3454,8 +3663,11 @@
       <c r="N66" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -3498,8 +3710,11 @@
       <c r="N67" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -3542,8 +3757,11 @@
       <c r="N68" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -3586,8 +3804,11 @@
       <c r="N69" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -3630,8 +3851,11 @@
       <c r="N70" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -3674,8 +3898,11 @@
       <c r="N71" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O71" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -3718,8 +3945,11 @@
       <c r="N72" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O72" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -3762,8 +3992,11 @@
       <c r="N73" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -3806,8 +4039,11 @@
       <c r="N74" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -3850,8 +4086,11 @@
       <c r="N75" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -3894,8 +4133,11 @@
       <c r="N76" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -3938,8 +4180,11 @@
       <c r="N77" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O77" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -3982,8 +4227,11 @@
       <c r="N78" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -4026,8 +4274,11 @@
       <c r="N79" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O79" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -4070,8 +4321,11 @@
       <c r="N80" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O80" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -4114,8 +4368,11 @@
       <c r="N81" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -4158,8 +4415,11 @@
       <c r="N82" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O82" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -4202,8 +4462,11 @@
       <c r="N83" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -4246,8 +4509,11 @@
       <c r="N84" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O84" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -4290,8 +4556,11 @@
       <c r="N85" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O85" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -4334,8 +4603,11 @@
       <c r="N86" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -4378,8 +4650,11 @@
       <c r="N87" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -4422,8 +4697,11 @@
       <c r="N88" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O88" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -4466,8 +4744,11 @@
       <c r="N89" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O89" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -4510,8 +4791,11 @@
       <c r="N90" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O90" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -4554,8 +4838,11 @@
       <c r="N91" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O91" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -4598,8 +4885,11 @@
       <c r="N92" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O92" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -4642,8 +4932,11 @@
       <c r="N93" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O93" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -4686,8 +4979,11 @@
       <c r="N94" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O94" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -4730,8 +5026,11 @@
       <c r="N95" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O95" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -4774,8 +5073,11 @@
       <c r="N96" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O96" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -4818,8 +5120,11 @@
       <c r="N97" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O97" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -4862,8 +5167,11 @@
       <c r="N98" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O98" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -4906,8 +5214,11 @@
       <c r="N99" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O99" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -4950,8 +5261,11 @@
       <c r="N100" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O100" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -4994,8 +5308,11 @@
       <c r="N101" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O101" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -5038,8 +5355,11 @@
       <c r="N102" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O102" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -5082,8 +5402,11 @@
       <c r="N103" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O103" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -5126,8 +5449,11 @@
       <c r="N104" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O104" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -5170,8 +5496,11 @@
       <c r="N105" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -5214,8 +5543,11 @@
       <c r="N106" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O106" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -5258,8 +5590,11 @@
       <c r="N107" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O107" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -5302,8 +5637,11 @@
       <c r="N108" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O108" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -5346,8 +5684,11 @@
       <c r="N109" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O109" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -5390,8 +5731,11 @@
       <c r="N110" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O110" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -5434,8 +5778,11 @@
       <c r="N111" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O111" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -5478,8 +5825,11 @@
       <c r="N112" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O112" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -5522,8 +5872,11 @@
       <c r="N113" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O113" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -5566,8 +5919,11 @@
       <c r="N114" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O114" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -5610,8 +5966,11 @@
       <c r="N115" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O115" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -5654,8 +6013,11 @@
       <c r="N116" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O116" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -5698,8 +6060,11 @@
       <c r="N117" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O117" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -5742,8 +6107,11 @@
       <c r="N118" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O118" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -5786,8 +6154,11 @@
       <c r="N119" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O119" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -5830,8 +6201,11 @@
       <c r="N120" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O120" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -5874,8 +6248,11 @@
       <c r="N121" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O121" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -5918,8 +6295,11 @@
       <c r="N122" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O122" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -5962,8 +6342,11 @@
       <c r="N123" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O123" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -6006,8 +6389,11 @@
       <c r="N124" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O124" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -6050,8 +6436,11 @@
       <c r="N125" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O125" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -6094,8 +6483,11 @@
       <c r="N126" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O126" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -6138,8 +6530,11 @@
       <c r="N127" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O127" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -6182,8 +6577,11 @@
       <c r="N128" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O128" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -6226,8 +6624,11 @@
       <c r="N129" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O129" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>1</v>
       </c>
@@ -6270,8 +6671,11 @@
       <c r="N130" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O130" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>1</v>
       </c>
@@ -6314,8 +6718,11 @@
       <c r="N131" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O131" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -6358,8 +6765,11 @@
       <c r="N132" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O132" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -6402,8 +6812,11 @@
       <c r="N133" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O133" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -6446,8 +6859,11 @@
       <c r="N134" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O134" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>1</v>
       </c>
@@ -6490,8 +6906,11 @@
       <c r="N135" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O135" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -6534,8 +6953,11 @@
       <c r="N136" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O136" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -6578,8 +7000,11 @@
       <c r="N137" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O137" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>1</v>
       </c>
@@ -6622,8 +7047,11 @@
       <c r="N138" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O138" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -6666,8 +7094,11 @@
       <c r="N139" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O139" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -6710,8 +7141,11 @@
       <c r="N140" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O140" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -6754,8 +7188,11 @@
       <c r="N141" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O141" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>1</v>
       </c>
@@ -6798,8 +7235,11 @@
       <c r="N142" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O142" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -6842,8 +7282,11 @@
       <c r="N143" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O143" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -6886,8 +7329,11 @@
       <c r="N144" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O144" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -6930,8 +7376,11 @@
       <c r="N145" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O145" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -6974,8 +7423,11 @@
       <c r="N146" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O146" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -7018,8 +7470,11 @@
       <c r="N147" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O147" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -7062,8 +7517,11 @@
       <c r="N148" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O148" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -7106,8 +7564,11 @@
       <c r="N149" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O149" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -7150,8 +7611,11 @@
       <c r="N150" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O150" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -7194,8 +7658,11 @@
       <c r="N151" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O151" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -7238,8 +7705,11 @@
       <c r="N152" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O152" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>1</v>
       </c>
@@ -7282,8 +7752,11 @@
       <c r="N153" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O153" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -7326,8 +7799,11 @@
       <c r="N154" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O154" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -7370,8 +7846,11 @@
       <c r="N155" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O155" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -7414,8 +7893,11 @@
       <c r="N156" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O156" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -7458,8 +7940,11 @@
       <c r="N157" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O157" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>1</v>
       </c>
@@ -7502,8 +7987,11 @@
       <c r="N158" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O158" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>1</v>
       </c>
@@ -7546,8 +8034,11 @@
       <c r="N159" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O159" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -7590,8 +8081,11 @@
       <c r="N160" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O160" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>1</v>
       </c>
@@ -7634,8 +8128,11 @@
       <c r="N161" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O161" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>1</v>
       </c>
@@ -7678,8 +8175,11 @@
       <c r="N162" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O162" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>1</v>
       </c>
@@ -7722,8 +8222,11 @@
       <c r="N163" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O163" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>1</v>
       </c>
@@ -7766,8 +8269,11 @@
       <c r="N164" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O164" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>1</v>
       </c>
@@ -7810,8 +8316,11 @@
       <c r="N165" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O165" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -7854,8 +8363,11 @@
       <c r="N166" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O166" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -7898,8 +8410,11 @@
       <c r="N167" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O167" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -7942,8 +8457,11 @@
       <c r="N168" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O168" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -7986,8 +8504,11 @@
       <c r="N169" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O169" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -8030,8 +8551,11 @@
       <c r="N170" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O170" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>1</v>
       </c>
@@ -8074,8 +8598,11 @@
       <c r="N171" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O171" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>1</v>
       </c>
@@ -8118,8 +8645,11 @@
       <c r="N172" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O172" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -8162,8 +8692,11 @@
       <c r="N173" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O173" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -8206,8 +8739,11 @@
       <c r="N174" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O174" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -8250,8 +8786,11 @@
       <c r="N175" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O175" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -8294,8 +8833,11 @@
       <c r="N176" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O176" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>1</v>
       </c>
@@ -8338,8 +8880,11 @@
       <c r="N177" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O177" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -8382,8 +8927,11 @@
       <c r="N178" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O178" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>1</v>
       </c>
@@ -8426,8 +8974,11 @@
       <c r="N179" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O179" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>1</v>
       </c>
@@ -8470,8 +9021,11 @@
       <c r="N180" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O180" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -8514,8 +9068,11 @@
       <c r="N181" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O181" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -8558,8 +9115,11 @@
       <c r="N182" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O182" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>1</v>
       </c>
@@ -8602,8 +9162,11 @@
       <c r="N183" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O183" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>1</v>
       </c>
@@ -8646,8 +9209,11 @@
       <c r="N184" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O184" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -8690,8 +9256,11 @@
       <c r="N185" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O185" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>1</v>
       </c>
@@ -8734,8 +9303,11 @@
       <c r="N186" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O186" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -8778,8 +9350,11 @@
       <c r="N187" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O187" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>1</v>
       </c>
@@ -8822,8 +9397,11 @@
       <c r="N188" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O188" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>1</v>
       </c>
@@ -8866,8 +9444,11 @@
       <c r="N189" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O189" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>1</v>
       </c>
@@ -8910,8 +9491,11 @@
       <c r="N190" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O190" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>1</v>
       </c>
@@ -8954,8 +9538,11 @@
       <c r="N191" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O191" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>1</v>
       </c>
@@ -8998,8 +9585,11 @@
       <c r="N192" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O192" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>1</v>
       </c>
@@ -9042,8 +9632,11 @@
       <c r="N193" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O193" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>1</v>
       </c>
@@ -9086,8 +9679,11 @@
       <c r="N194" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O194" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>1</v>
       </c>
@@ -9130,8 +9726,11 @@
       <c r="N195" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O195" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -9174,8 +9773,11 @@
       <c r="N196" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O196" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -9218,8 +9820,11 @@
       <c r="N197" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O197" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -9262,8 +9867,11 @@
       <c r="N198" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O198" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>1</v>
       </c>
@@ -9306,8 +9914,11 @@
       <c r="N199" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O199" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -9350,8 +9961,11 @@
       <c r="N200" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O200" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>1</v>
       </c>
@@ -9393,6 +10007,9 @@
       </c>
       <c r="N201" t="s">
         <v>1</v>
+      </c>
+      <c r="O201" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>